<commit_message>
update scripts' streamline process
replace template to correct one; add a config file storing all paths of script; add test scripts to check integrity of files
</commit_message>
<xml_diff>
--- a/data_raw/Template_for_Adding_Courses_to_Sustainability_Course_Finder.xlsx
+++ b/data_raw/Template_for_Adding_Courses_to_Sustainability_Course_Finder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliehopper/Dropbox/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\SustainabilityCourseFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA35568-6B8A-BD42-B1DE-D7D243189082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD92707-8B2C-4F2F-BBC7-0EAB03730052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{3E9B7C92-6739-1340-9EDD-02531B8302F5}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="8170" xr2:uid="{3E9B7C92-6739-1340-9EDD-02531B8302F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Andrew and Erna Viterbi School of Engineering</t>
   </si>
@@ -44,12 +44,6 @@
     <t>ENGR-499</t>
   </si>
   <si>
-    <t>Special Topics: Systems Thinking for Sustainability</t>
-  </si>
-  <si>
-    <t>Albright, Julie; Maby, Edward</t>
-  </si>
-  <si>
     <t>SP24</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
     <t>semester</t>
   </si>
   <si>
-    <t>course_desc</t>
-  </si>
-  <si>
     <t>department</t>
   </si>
   <si>
@@ -92,9 +83,6 @@
     <t>course_level</t>
   </si>
   <si>
-    <t>Special Topics: Systems Thinking for Sustainability- This course will grow your understanding about the foundational systems shaping our world - energy, communications, transportation, water, waste, mining, and others - emphasizing their intersection (a "systems approach") with the social, environmental, business, policy, and technical arenas.</t>
-  </si>
-  <si>
     <t>Data_Instructions</t>
   </si>
   <si>
@@ -107,37 +95,58 @@
     <t>AME-599</t>
   </si>
   <si>
-    <t>Special Topic: Sustainable Aerospace</t>
-  </si>
-  <si>
     <t>Bradley, Marty</t>
   </si>
   <si>
-    <t>29085R</t>
-  </si>
-  <si>
-    <t>FA24</t>
-  </si>
-  <si>
     <t>graduate</t>
   </si>
   <si>
-    <t xml:space="preserve">Special Topics: This course presents the history and current developments in the field of sustainable aerospace, covering both aviation and space topics. Topics will include alternative fuels (biofuels, synthetic fuels, methane, alcohols, and hydrogen), electric and hybrid electric aircraft, lifecycle environmental impact and analysis, space debris, the environmental impact of rocket launches and space debris reentry, and aerospace technology based ideas to mitigate climate change.  The advantages and challenges of each type of potential sustainable aerospace technology will be discussed, evaluated, and compared. </t>
-  </si>
-  <si>
     <t>AME-499</t>
   </si>
   <si>
-    <t>Special Topic: Sustainable Aviation</t>
-  </si>
-  <si>
-    <t>Special Topics: This course presents the history and current developments in the field of sustainable aviation. Topics will include alternative fuels (biofuels, synthetic fuels, methane, alcohols, and hydrogen), electric and hybrid electric aircraft, and lifecycle environmental impact and analysis.  The advantages and challenges of each type of potential sustainable aviation technology will be discussed, evaluated, and compared.  The target audience for this course is undergraduate and graduate students with an interest or background in aerospace engineering or sustainable energy who want to learn about sustainable aviation.</t>
-  </si>
-  <si>
-    <t>29035R</t>
-  </si>
-  <si>
     <t>AY25</t>
+  </si>
+  <si>
+    <t>F24</t>
+  </si>
+  <si>
+    <t>section_name</t>
+  </si>
+  <si>
+    <t>Special Topics</t>
+  </si>
+  <si>
+    <t>Systems Thinking for Sustainability</t>
+  </si>
+  <si>
+    <t>Sustainable Aerospace</t>
+  </si>
+  <si>
+    <t>Sustainable Aviation</t>
+  </si>
+  <si>
+    <t>course_description</t>
+  </si>
+  <si>
+    <t>This course will grow your understanding about the foundational systems shaping our world - energy, communications, transportation, water, waste, mining, and others - emphasizing their intersection (a "systems approach") with the social, environmental, business, policy, and technical arenas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This course presents the history and current developments in the field of sustainable aerospace, covering both aviation and space topics. Topics will include alternative fuels (biofuels, synthetic fuels, methane, alcohols, and hydrogen), electric and hybrid electric aircraft, lifecycle environmental impact and analysis, space debris, the environmental impact of rocket launches and space debris reentry, and aerospace technology based ideas to mitigate climate change.  The advantages and challenges of each type of potential sustainable aerospace technology will be discussed, evaluated, and compared. </t>
+  </si>
+  <si>
+    <t>This course presents the history and current developments in the field of sustainable aviation. Topics will include alternative fuels (biofuels, synthetic fuels, methane, alcohols, and hydrogen), electric and hybrid electric aircraft, and lifecycle environmental impact and analysis.  The advantages and challenges of each type of potential sustainable aviation technology will be discussed, evaluated, and compared.  The target audience for this course is undergraduate and graduate students with an interest or background in aerospace engineering or sustainable energy who want to learn about sustainable aviation.</t>
+  </si>
+  <si>
+    <t>Albright, Julie;Maby, Edward, W</t>
+  </si>
+  <si>
+    <t>ENGR</t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>Update Description</t>
   </si>
 </sst>
 </file>
@@ -260,9 +269,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -300,7 +309,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -406,7 +415,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -548,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -556,169 +565,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B90C02-862D-8944-8647-8139FC139BF2}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.83203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" style="5"/>
     <col min="3" max="3" width="16" style="5" customWidth="1"/>
-    <col min="4" max="8" width="11.1640625" style="5"/>
-    <col min="9" max="9" width="75.1640625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" style="5"/>
-    <col min="12" max="12" width="15.5" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="11.1640625" style="5"/>
+    <col min="4" max="9" width="11.1640625" style="5"/>
+    <col min="10" max="10" width="75.1640625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="5" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" style="5"/>
+    <col min="13" max="13" width="15.5" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="11.1640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
+      <c r="N1" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="4">
+        <v>28535</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4">
-        <v>28535</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="5">
+        <v>29085</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="5">
-        <v>1</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>27</v>
+      <c r="M3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="5">
+        <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="E4" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="7">
+        <v>29035</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="7">
+      <c r="K4" s="7">
         <v>1</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="L4" s="7" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="7">
+        <v>966</v>
       </c>
     </row>
   </sheetData>

</xml_diff>